<commit_message>
Huiswerk toegevoegd week 4, en ontwerpen in groepen opdracht begin gemaakt
</commit_message>
<xml_diff>
--- a/Ontwerpen in groepen/Opdracht week 4 en 5/Methodisch Ontwerpen Werkbladen Excel V1.0.xlsx
+++ b/Ontwerpen in groepen/Opdracht week 4 en 5/Methodisch Ontwerpen Werkbladen Excel V1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mechatronica-2024\Ontwerpen in groepen\Opdracht week 4 en 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\HBO-Mechatronica-Jaar-1-2024\Ontwerpen in groepen\Opdracht week 4 en 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08079A3A-8588-4180-AADE-0A75E45E9482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5A1ECC0-94AD-411C-8CAE-30A45217AD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lijst van Eisen" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Functies</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Werkwijzen</t>
   </si>
   <si>
-    <t>Hoofdfunctie</t>
-  </si>
-  <si>
     <t>Deelfuncties</t>
   </si>
   <si>
@@ -144,13 +141,82 @@
   </si>
   <si>
     <t>Hoe kun je …………………………………………………………………..……………?</t>
+  </si>
+  <si>
+    <t>De robot moet kunnen rijden</t>
+  </si>
+  <si>
+    <t>De robot moet kunnen draaien</t>
+  </si>
+  <si>
+    <t>De robot moet kunnen aanvallen</t>
+  </si>
+  <si>
+    <t>De robot moet kunnen incasseren</t>
+  </si>
+  <si>
+    <t>De robot moet bestuurbaar zijn</t>
+  </si>
+  <si>
+    <t>De robot moet zonder externe stroom werken</t>
+  </si>
+  <si>
+    <t>De robot moet stabiel blijven staan</t>
+  </si>
+  <si>
+    <t>De robot moet een sterk exterieur hebben</t>
+  </si>
+  <si>
+    <t>De robot moet wielen hebben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De robot moet één of meer wapens hebben </t>
+  </si>
+  <si>
+    <t>De robot moet rupsbanden hebben</t>
+  </si>
+  <si>
+    <t>De robor moet een motor hebben</t>
+  </si>
+  <si>
+    <t>De robot moet een batterij hebben</t>
+  </si>
+  <si>
+    <t>Rijden</t>
+  </si>
+  <si>
+    <t>Draaien</t>
+  </si>
+  <si>
+    <t>Aanvallen</t>
+  </si>
+  <si>
+    <t>Incasseren</t>
+  </si>
+  <si>
+    <t>Besturen</t>
+  </si>
+  <si>
+    <t>Stabbiliseren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoofdfunctie </t>
+  </si>
+  <si>
+    <t>Langer blijven staan dan de robot van de tegenstander</t>
+  </si>
+  <si>
+    <t>Zelf voorzienen van  energie</t>
+  </si>
+  <si>
+    <t>Rijden, draaien, aanvallen, incasseren besturen, zelf voorzien van energie, stabilliseren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +241,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -382,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -475,9 +548,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,6 +572,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -760,88 +859,116 @@
   </sheetPr>
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="152.5546875" customWidth="1"/>
+    <col min="1" max="1" width="152.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-    </row>
-    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-    </row>
-    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-    </row>
-    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-    </row>
-    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-    </row>
-    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-    </row>
-    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-    </row>
-    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-    </row>
-    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-    </row>
-    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
-    </row>
-    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-    </row>
-    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-    </row>
-    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-    </row>
-    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="35"/>
     </row>
-    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="35"/>
     </row>
-    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="35"/>
     </row>
-    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="35"/>
     </row>
-    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="35"/>
     </row>
-    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="35"/>
     </row>
-    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="35"/>
     </row>
-    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="35"/>
     </row>
-    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="35"/>
     </row>
-    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="35"/>
     </row>
-    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="35"/>
     </row>
   </sheetData>
@@ -857,164 +984,330 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="2" width="7.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="72.44140625" style="2" customWidth="1"/>
-    <col min="4" max="6" width="7.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="2" width="7.68359375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.41796875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="7.68359375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:8" ht="74.400000000000006" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="2" spans="1:8" ht="72.3" x14ac:dyDescent="0.75">
       <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A8" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A12" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A13" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A14" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A15" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A16" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="D16" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="H16" s="11"/>
     </row>
   </sheetData>
@@ -1030,90 +1323,104 @@
   </sheetPr>
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="152.5546875" customWidth="1"/>
+    <col min="1" max="1" width="152.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-    </row>
-    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-    </row>
-    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-    </row>
-    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-    </row>
-    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-    </row>
-    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-    </row>
-    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-    </row>
-    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="35"/>
     </row>
-    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="35"/>
     </row>
-    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="35"/>
     </row>
-    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="35"/>
     </row>
-    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="35"/>
     </row>
-    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="35"/>
     </row>
-    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="35"/>
     </row>
-    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="35"/>
     </row>
-    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="35"/>
     </row>
-    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="35"/>
     </row>
-    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="35"/>
     </row>
-    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="35"/>
     </row>
-    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="35"/>
     </row>
-    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="35"/>
     </row>
-    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="35"/>
     </row>
-    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="35"/>
     </row>
-    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="35"/>
     </row>
   </sheetData>
@@ -1127,27 +1434,73 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="144.109375" customWidth="1"/>
+    <col min="1" max="1" width="144.15625" customWidth="1"/>
+    <col min="2" max="2" width="91" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:1" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="3.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:2" ht="96.75" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="405" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="405" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="45"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="45"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="45"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="45"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="45"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="45"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="45"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="45"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="45"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="45"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="45"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="45"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1162,22 +1515,22 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="144.109375" customWidth="1"/>
+    <col min="1" max="1" width="144.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:1" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="3.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:1" ht="96.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="405" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="405" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="36"/>
     </row>
   </sheetData>
@@ -1197,14 +1550,14 @@
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="11.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1574,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="37"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -1254,9 +1607,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1269,9 +1622,9 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1284,9 +1637,9 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1299,9 +1652,9 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1314,9 +1667,9 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1329,9 +1682,9 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1344,9 +1697,9 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1359,7 +1712,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1372,7 +1725,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1385,7 +1738,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1414,46 +1767,46 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="72" customWidth="1"/>
-    <col min="2" max="7" width="6.6640625" customWidth="1"/>
+    <col min="2" max="7" width="6.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="48.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:10" ht="47.1" x14ac:dyDescent="0.75">
       <c r="A2" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>25</v>
-      </c>
       <c r="G2" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="11"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A3" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="3"/>
@@ -1465,12 +1818,12 @@
       <c r="I3" s="11"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A4" s="25">
         <v>1</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1481,13 +1834,13 @@
       <c r="I4" s="11"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A5" s="25">
         <v>2</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1497,14 +1850,14 @@
       <c r="I5" s="11"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A6" s="25">
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1513,7 +1866,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A7" s="25">
         <v>4</v>
       </c>
@@ -1521,7 +1874,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="30"/>
@@ -1529,7 +1882,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A8" s="25">
         <v>5</v>
       </c>
@@ -1538,16 +1891,16 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="30"/>
       <c r="H8" s="2"/>
       <c r="I8" s="11"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A9" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1559,12 +1912,12 @@
       <c r="I9" s="11"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A10" s="25">
         <v>1</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1575,13 +1928,13 @@
       <c r="I10" s="11"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A11" s="25">
         <v>2</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1591,14 +1944,14 @@
       <c r="I11" s="11"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A12" s="25">
         <v>3</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1607,7 +1960,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A13" s="25">
         <v>4</v>
       </c>
@@ -1615,7 +1968,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="30"/>
@@ -1623,7 +1976,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A14" s="25">
         <v>5</v>
       </c>
@@ -1632,7 +1985,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="30"/>
       <c r="H14" s="2"/>
@@ -1659,40 +2012,40 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" customWidth="1"/>
-    <col min="2" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.41796875" customWidth="1"/>
+    <col min="2" max="5" width="7.68359375" customWidth="1"/>
+    <col min="6" max="6" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.578125" customWidth="1"/>
+    <col min="8" max="8" width="9.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:7" ht="72.599999999999994" x14ac:dyDescent="0.75">
       <c r="A2" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A3" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="3"/>
@@ -1701,7 +2054,7 @@
       <c r="F3" s="30"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A4" s="25">
         <v>1</v>
       </c>
@@ -1712,7 +2065,7 @@
       <c r="F4" s="30"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A5" s="25">
         <v>2</v>
       </c>
@@ -1723,7 +2076,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A6" s="25">
         <v>3</v>
       </c>
@@ -1734,7 +2087,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A7" s="25">
         <v>4</v>
       </c>
@@ -1745,7 +2098,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A8" s="25">
         <v>5</v>
       </c>
@@ -1756,9 +2109,9 @@
       <c r="F8" s="30"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A9" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="39"/>
       <c r="C9" s="3"/>
@@ -1767,28 +2120,28 @@
       <c r="F9" s="30"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A10" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="41"/>
       <c r="C10" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="32">
         <v>1</v>
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A11" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1797,7 +2150,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A12" s="25">
         <v>1</v>
       </c>
@@ -1808,7 +2161,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A13" s="25">
         <v>2</v>
       </c>
@@ -1819,7 +2172,7 @@
       <c r="F13" s="30"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A14" s="25">
         <v>3</v>
       </c>
@@ -1830,7 +2183,7 @@
       <c r="F14" s="30"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A15" s="25">
         <v>4</v>
       </c>
@@ -1841,7 +2194,7 @@
       <c r="F15" s="30"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A16" s="25">
         <v>5</v>
       </c>
@@ -1852,9 +2205,9 @@
       <c r="F16" s="30"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A17" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="39"/>
       <c r="C17" s="3"/>
@@ -1863,19 +2216,19 @@
       <c r="F17" s="30"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A18" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="32">
         <v>1</v>
@@ -1905,16 +2258,16 @@
       <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="24" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="24" width="5.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="15">
         <v>1</v>
@@ -1930,7 +2283,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="23"/>
     </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="42"/>
       <c r="B3" s="16"/>
       <c r="C3" s="13"/>
@@ -1944,7 +2297,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="42"/>
       <c r="B4" s="15">
         <v>0.8</v>
@@ -1960,7 +2313,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="42"/>
       <c r="B5" s="16"/>
       <c r="C5" s="13"/>
@@ -1974,7 +2327,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="42"/>
       <c r="B6" s="15">
         <v>0.6</v>
@@ -1990,7 +2343,7 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="42"/>
       <c r="B7" s="16"/>
       <c r="C7" s="13"/>
@@ -2004,7 +2357,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
     </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="42"/>
       <c r="B8" s="15">
         <v>0.4</v>
@@ -2020,7 +2373,7 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="42"/>
       <c r="B9" s="16"/>
       <c r="C9" s="13"/>
@@ -2034,7 +2387,7 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="42"/>
       <c r="B10" s="15">
         <v>0.2</v>
@@ -2050,7 +2403,7 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="42"/>
       <c r="B11" s="16"/>
       <c r="C11" s="23"/>
@@ -2064,7 +2417,7 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="42"/>
       <c r="B12" s="17">
         <v>0</v>
@@ -2085,9 +2438,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="B13" s="43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>

</xml_diff>